<commit_message>
change reporter generator; add CONF4 to PSO
</commit_message>
<xml_diff>
--- a/results/ga-overall-comparison.xlsx
+++ b/results/ga-overall-comparison.xlsx
@@ -367,13 +367,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0345</c:v>
+                    <c:v>0.094</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0948</c:v>
+                    <c:v>0.1473</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.022</c:v>
+                    <c:v>0.0525</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -385,13 +385,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0345</c:v>
+                    <c:v>0.094</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0948</c:v>
+                    <c:v>0.1473</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.022</c:v>
+                    <c:v>0.0525</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -434,13 +434,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.7008</c:v>
+                  <c:v>0.6695</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6694</c:v>
+                  <c:v>0.6873</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5899</c:v>
+                  <c:v>0.5791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,11 +456,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="886255600"/>
-        <c:axId val="909406240"/>
+        <c:axId val="-777932064"/>
+        <c:axId val="-700703648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="886255600"/>
+        <c:axId val="-777932064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,7 +503,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="909406240"/>
+        <c:crossAx val="-700703648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -511,7 +511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="909406240"/>
+        <c:axId val="-700703648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,7 +561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="886255600"/>
+        <c:crossAx val="-777932064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1486,7 +1486,7 @@
   <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,13 +1524,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.70079999999999998</v>
+        <v>0.66949999999999998</v>
       </c>
       <c r="D4">
-        <v>0.6694</v>
+        <v>0.68730000000000002</v>
       </c>
       <c r="F4">
-        <v>0.58989999999999998</v>
+        <v>0.57909999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1552,13 +1552,13 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>3.4500000000000003E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D7">
-        <v>9.4799999999999995E-2</v>
+        <v>0.14729999999999999</v>
       </c>
       <c r="F7">
-        <v>2.1999999999999999E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>